<commit_message>
fix store country name in template
</commit_message>
<xml_diff>
--- a/Projects/HEINZCR/Config/sub_category_scores_v1.xlsx
+++ b/Projects/HEINZCR/Config/sub_category_scores_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="category_score" sheetId="1" state="visible" r:id="rId2"/>
@@ -35,16 +35,16 @@
     <t xml:space="preserve">Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">T&amp;T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTM</t>
+    <t xml:space="preserve">Trinidad &amp; Tobago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jamaica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puerto Rico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guatemala</t>
   </si>
   <si>
     <t xml:space="preserve">Ketchup</t>
@@ -287,8 +287,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -296,7 +296,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +528,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Columbia targets to sub_category_scores_v1.xlsx
</commit_message>
<xml_diff>
--- a/Projects/HEINZCR/Config/sub_category_scores_v1.xlsx
+++ b/Projects/HEINZCR/Config/sub_category_scores_v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="category_score" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">Guatemala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columbia</t>
   </si>
   <si>
     <t xml:space="preserve">Ketchup</t>
@@ -285,19 +288,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.9132653061225"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -322,130 +324,146 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -453,13 +471,14 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -468,26 +487,28 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>7.5</v>
@@ -508,6 +529,9 @@
         <v>7.5</v>
       </c>
       <c r="H12" s="3" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I12" s="3" t="n">
         <v>7.5</v>
       </c>
     </row>
@@ -534,18 +558,21 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>3</v>
@@ -553,7 +580,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>3</v>
@@ -561,7 +588,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>1</v>
@@ -569,7 +596,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>3</v>
@@ -577,7 +604,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Update score execution values
</commit_message>
<xml_diff>
--- a/Projects/HEINZCR/Config/sub_category_scores_v1.xlsx
+++ b/Projects/HEINZCR/Config/sub_category_scores_v1.xlsx
@@ -291,12 +291,12 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.9132653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.6887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -506,24 +506,24 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>7.5</v>
+        <v>5.1</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>7.5</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>7.5</v>
+        <v>6.2</v>
       </c>
       <c r="G12" s="3" t="n">
         <v>7.5</v>
@@ -532,7 +532,7 @@
         <v>7.5</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>7.5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -559,7 +559,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>